<commit_message>
added crs check; filled in shapefilekarteringinfo
</commit_message>
<xml_diff>
--- a/data/Overzicht_vegetatiekarteringen.xlsx
+++ b/data/Overzicht_vegetatiekarteringen.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\jordydelange\git\veg2hab\testing\vegetatiekarteringen\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\jordydelange\git\veg2hab\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{479C79FA-F1DA-4862-9380-E13FCEFEC7E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ABB8C2E-0059-468F-9E97-B8078804FE3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4380" yWindow="3840" windowWidth="25845" windowHeight="16665" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="27885" yWindow="1365" windowWidth="14985" windowHeight="15750" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Vegetatiekarteringen" sheetId="1" r:id="rId1"/>
@@ -587,9 +587,6 @@
     <t>Drouwenerzand_2020</t>
   </si>
   <si>
-    <t>/DR Extra/2020_Drouwenerzand/HDL_Drouwenerzand_2020.shp</t>
-  </si>
-  <si>
     <t>NM_Mantingerbos_2015</t>
   </si>
   <si>
@@ -1089,6 +1086,9 @@
   </si>
   <si>
     <t>./FR Extra/2022_Bakkefean/GISbestanden/vlakken.shp</t>
+  </si>
+  <si>
+    <t>./DR Extra/2020_Drouwenerzand/HDL_Drouwenerzand_2020.shp</t>
   </si>
 </sst>
 </file>
@@ -1527,16 +1527,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J81"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.5703125" customWidth="1"/>
-    <col min="2" max="2" width="29.85546875" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="2" max="2" width="56.28515625" customWidth="1"/>
+    <col min="3" max="3" width="68.42578125" customWidth="1"/>
     <col min="4" max="4" width="6.42578125" customWidth="1"/>
     <col min="5" max="5" width="18.7109375" customWidth="1"/>
     <col min="6" max="6" width="15.42578125" customWidth="1"/>
@@ -2895,7 +2895,7 @@
         <v>139</v>
       </c>
       <c r="C45" t="s">
-        <v>140</v>
+        <v>307</v>
       </c>
       <c r="D45" t="s">
         <v>13</v>
@@ -2921,10 +2921,10 @@
         <v>86</v>
       </c>
       <c r="B46" t="s">
+        <v>140</v>
+      </c>
+      <c r="C46" t="s">
         <v>141</v>
-      </c>
-      <c r="C46" t="s">
-        <v>142</v>
       </c>
       <c r="D46" t="s">
         <v>13</v>
@@ -2947,19 +2947,19 @@
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
+        <v>142</v>
+      </c>
+      <c r="B47" t="s">
         <v>143</v>
       </c>
-      <c r="B47" t="s">
+      <c r="C47" t="s">
         <v>144</v>
       </c>
-      <c r="C47" t="s">
+      <c r="D47" t="s">
+        <v>13</v>
+      </c>
+      <c r="E47" t="s">
         <v>145</v>
-      </c>
-      <c r="D47" t="s">
-        <v>13</v>
-      </c>
-      <c r="E47" t="s">
-        <v>146</v>
       </c>
       <c r="F47" t="s">
         <v>40</v>
@@ -2974,50 +2974,50 @@
         <v>13</v>
       </c>
       <c r="J47" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="48" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="B48" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="B48" s="4" t="s">
-        <v>144</v>
-      </c>
       <c r="C48" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="D48" s="4" t="s">
         <v>148</v>
-      </c>
-      <c r="D48" s="4" t="s">
-        <v>149</v>
       </c>
       <c r="E48" s="4" t="s">
         <v>14</v>
       </c>
       <c r="F48" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="G48" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H48" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I48" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J48" s="4" t="s">
         <v>150</v>
-      </c>
-      <c r="G48" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H48" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="I48" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J48" s="4" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B49" t="s">
+        <v>151</v>
+      </c>
+      <c r="C49" t="s">
         <v>152</v>
-      </c>
-      <c r="C49" t="s">
-        <v>153</v>
       </c>
       <c r="D49" t="s">
         <v>13</v>
@@ -3038,18 +3038,18 @@
         <v>16</v>
       </c>
       <c r="J49" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B50" t="s">
+        <v>154</v>
+      </c>
+      <c r="C50" t="s">
         <v>155</v>
-      </c>
-      <c r="C50" t="s">
-        <v>156</v>
       </c>
       <c r="D50" t="s">
         <v>13</v>
@@ -3070,18 +3070,18 @@
         <v>16</v>
       </c>
       <c r="J50" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B51" t="s">
+        <v>157</v>
+      </c>
+      <c r="C51" t="s">
         <v>158</v>
-      </c>
-      <c r="C51" t="s">
-        <v>159</v>
       </c>
       <c r="D51" t="s">
         <v>13</v>
@@ -3102,24 +3102,24 @@
         <v>16</v>
       </c>
       <c r="J51" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="52" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B52" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="C52" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="C52" s="4" t="s">
+      <c r="D52" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E52" s="4" t="s">
         <v>162</v>
-      </c>
-      <c r="D52" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E52" s="4" t="s">
-        <v>163</v>
       </c>
       <c r="F52" s="4" t="s">
         <v>40</v>
@@ -3134,18 +3134,18 @@
         <v>16</v>
       </c>
       <c r="J52" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B53" t="s">
+        <v>164</v>
+      </c>
+      <c r="C53" t="s">
         <v>165</v>
-      </c>
-      <c r="C53" t="s">
-        <v>166</v>
       </c>
       <c r="D53" t="s">
         <v>13</v>
@@ -3166,18 +3166,18 @@
         <v>16</v>
       </c>
       <c r="J53" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B54" t="s">
+        <v>167</v>
+      </c>
+      <c r="C54" t="s">
         <v>168</v>
-      </c>
-      <c r="C54" t="s">
-        <v>169</v>
       </c>
       <c r="D54" t="s">
         <v>13</v>
@@ -3192,24 +3192,24 @@
         <v>13</v>
       </c>
       <c r="H54" t="s">
+        <v>169</v>
+      </c>
+      <c r="I54" t="s">
+        <v>16</v>
+      </c>
+      <c r="J54" t="s">
         <v>170</v>
-      </c>
-      <c r="I54" t="s">
-        <v>16</v>
-      </c>
-      <c r="J54" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B55" t="s">
+        <v>171</v>
+      </c>
+      <c r="C55" t="s">
         <v>172</v>
-      </c>
-      <c r="C55" t="s">
-        <v>173</v>
       </c>
       <c r="D55" t="s">
         <v>13</v>
@@ -3230,18 +3230,18 @@
         <v>16</v>
       </c>
       <c r="J55" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B56" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C56" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D56" t="s">
         <v>13</v>
@@ -3262,18 +3262,18 @@
         <v>16</v>
       </c>
       <c r="J56" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B57" t="s">
+        <v>176</v>
+      </c>
+      <c r="C57" t="s">
         <v>177</v>
-      </c>
-      <c r="C57" t="s">
-        <v>178</v>
       </c>
       <c r="D57" t="s">
         <v>13</v>
@@ -3294,50 +3294,50 @@
         <v>16</v>
       </c>
       <c r="J57" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B58" t="s">
+        <v>179</v>
+      </c>
+      <c r="C58" t="s">
         <v>180</v>
       </c>
-      <c r="C58" t="s">
+      <c r="D58" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E58" t="s">
+        <v>145</v>
+      </c>
+      <c r="F58" t="s">
         <v>181</v>
       </c>
-      <c r="D58" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E58" t="s">
-        <v>146</v>
-      </c>
-      <c r="F58" t="s">
+      <c r="G58" t="s">
+        <v>13</v>
+      </c>
+      <c r="H58" t="s">
+        <v>13</v>
+      </c>
+      <c r="I58" t="s">
+        <v>16</v>
+      </c>
+      <c r="J58" s="2" t="s">
         <v>182</v>
-      </c>
-      <c r="G58" t="s">
-        <v>13</v>
-      </c>
-      <c r="H58" t="s">
-        <v>13</v>
-      </c>
-      <c r="I58" t="s">
-        <v>16</v>
-      </c>
-      <c r="J58" s="2" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B59" t="s">
+        <v>183</v>
+      </c>
+      <c r="C59" t="s">
         <v>184</v>
-      </c>
-      <c r="C59" t="s">
-        <v>185</v>
       </c>
       <c r="D59" t="s">
         <v>13</v>
@@ -3360,13 +3360,13 @@
     </row>
     <row r="60" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B60" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="C60" s="4" t="s">
         <v>186</v>
-      </c>
-      <c r="C60" s="4" t="s">
-        <v>187</v>
       </c>
       <c r="D60" s="4" t="s">
         <v>13</v>
@@ -3387,18 +3387,18 @@
         <v>16</v>
       </c>
       <c r="J60" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B61" t="s">
+        <v>188</v>
+      </c>
+      <c r="C61" t="s">
         <v>189</v>
-      </c>
-      <c r="C61" t="s">
-        <v>190</v>
       </c>
       <c r="D61" t="s">
         <v>13</v>
@@ -3421,13 +3421,13 @@
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B62" t="s">
+        <v>190</v>
+      </c>
+      <c r="C62" t="s">
         <v>191</v>
-      </c>
-      <c r="C62" t="s">
-        <v>192</v>
       </c>
       <c r="D62" t="s">
         <v>13</v>
@@ -3450,13 +3450,13 @@
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B63" t="s">
+        <v>192</v>
+      </c>
+      <c r="C63" t="s">
         <v>193</v>
-      </c>
-      <c r="C63" t="s">
-        <v>194</v>
       </c>
       <c r="D63" t="s">
         <v>13</v>
@@ -3479,13 +3479,13 @@
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B64" t="s">
+        <v>194</v>
+      </c>
+      <c r="C64" t="s">
         <v>195</v>
-      </c>
-      <c r="C64" t="s">
-        <v>196</v>
       </c>
       <c r="D64" t="s">
         <v>13</v>
@@ -3506,18 +3506,18 @@
         <v>16</v>
       </c>
       <c r="J64" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
+        <v>197</v>
+      </c>
+      <c r="B65" t="s">
         <v>198</v>
       </c>
-      <c r="B65" t="s">
-        <v>199</v>
-      </c>
       <c r="C65" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D65" t="s">
         <v>13</v>
@@ -3540,13 +3540,13 @@
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B66" t="s">
+        <v>199</v>
+      </c>
+      <c r="C66" t="s">
         <v>200</v>
-      </c>
-      <c r="C66" t="s">
-        <v>201</v>
       </c>
       <c r="D66" t="s">
         <v>13</v>
@@ -3569,13 +3569,13 @@
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B67" t="s">
+        <v>201</v>
+      </c>
+      <c r="C67" t="s">
         <v>202</v>
-      </c>
-      <c r="C67" t="s">
-        <v>203</v>
       </c>
       <c r="D67" t="s">
         <v>13</v>
@@ -3598,13 +3598,13 @@
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B68" t="s">
+        <v>203</v>
+      </c>
+      <c r="C68" t="s">
         <v>204</v>
-      </c>
-      <c r="C68" t="s">
-        <v>205</v>
       </c>
       <c r="D68" t="s">
         <v>13</v>
@@ -3625,18 +3625,18 @@
         <v>16</v>
       </c>
       <c r="J68" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B69" t="s">
+        <v>206</v>
+      </c>
+      <c r="C69" t="s">
         <v>207</v>
-      </c>
-      <c r="C69" t="s">
-        <v>208</v>
       </c>
       <c r="D69" t="s">
         <v>13</v>
@@ -3659,36 +3659,36 @@
     </row>
     <row r="70" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B70" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="C70" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="C70" s="4" t="s">
+      <c r="D70" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J70" s="4" t="s">
         <v>210</v>
-      </c>
-      <c r="D70" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J70" s="4" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="71" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="B71" s="4" t="s">
         <v>212</v>
       </c>
-      <c r="B71" s="4" t="s">
+      <c r="C71" s="4" t="s">
         <v>213</v>
       </c>
-      <c r="C71" s="4" t="s">
-        <v>214</v>
-      </c>
       <c r="D71" s="4" t="s">
         <v>16</v>
       </c>
       <c r="E71" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F71" s="4" t="s">
         <v>40</v>
@@ -3703,18 +3703,18 @@
         <v>16</v>
       </c>
       <c r="J71" s="4" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B72" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C72" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D72" t="s">
         <v>13</v>
@@ -3735,18 +3735,18 @@
         <v>13</v>
       </c>
       <c r="J72" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B73" t="s">
+        <v>217</v>
+      </c>
+      <c r="C73" t="s">
         <v>218</v>
-      </c>
-      <c r="C73" t="s">
-        <v>219</v>
       </c>
       <c r="D73" t="s">
         <v>13</v>
@@ -3767,18 +3767,18 @@
         <v>16</v>
       </c>
       <c r="J73" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B74" t="s">
+        <v>220</v>
+      </c>
+      <c r="C74" t="s">
         <v>221</v>
-      </c>
-      <c r="C74" t="s">
-        <v>222</v>
       </c>
       <c r="D74" t="s">
         <v>13</v>
@@ -3802,13 +3802,13 @@
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B75" t="s">
+        <v>222</v>
+      </c>
+      <c r="C75" t="s">
         <v>223</v>
-      </c>
-      <c r="C75" t="s">
-        <v>224</v>
       </c>
       <c r="D75" t="s">
         <v>13</v>
@@ -3831,13 +3831,13 @@
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B76" t="s">
+        <v>224</v>
+      </c>
+      <c r="C76" t="s">
         <v>225</v>
-      </c>
-      <c r="C76" t="s">
-        <v>226</v>
       </c>
       <c r="D76" t="s">
         <v>13</v>
@@ -3858,18 +3858,18 @@
         <v>13</v>
       </c>
       <c r="J76" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B77" t="s">
+        <v>226</v>
+      </c>
+      <c r="C77" t="s">
         <v>227</v>
-      </c>
-      <c r="C77" t="s">
-        <v>228</v>
       </c>
       <c r="D77" t="s">
         <v>13</v>
@@ -3892,13 +3892,13 @@
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B78" t="s">
+        <v>228</v>
+      </c>
+      <c r="C78" t="s">
         <v>229</v>
-      </c>
-      <c r="C78" t="s">
-        <v>230</v>
       </c>
       <c r="D78" t="s">
         <v>13</v>
@@ -3919,18 +3919,18 @@
         <v>13</v>
       </c>
       <c r="J78" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B79" t="s">
+        <v>231</v>
+      </c>
+      <c r="C79" t="s">
         <v>232</v>
-      </c>
-      <c r="C79" t="s">
-        <v>233</v>
       </c>
       <c r="D79" t="s">
         <v>13</v>
@@ -3953,39 +3953,39 @@
     </row>
     <row r="80" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80" s="4" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B80" s="4" t="s">
+        <v>233</v>
+      </c>
+      <c r="C80" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="C80" s="4" t="s">
+      <c r="D80" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G80" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H80" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I80" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J80" s="4" t="s">
         <v>235</v>
-      </c>
-      <c r="D80" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G80" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H80" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="I80" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J80" s="4" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="81" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="4" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B81" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="C81" s="4" t="s">
         <v>237</v>
-      </c>
-      <c r="C81" s="4" t="s">
-        <v>238</v>
       </c>
       <c r="D81" s="4" t="s">
         <v>13</v>
@@ -3994,25 +3994,26 @@
         <v>66</v>
       </c>
       <c r="F81" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="G81" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H81" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I81" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J81" s="4" t="s">
         <v>239</v>
-      </c>
-      <c r="G81" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H81" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="I81" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J81" s="4" t="s">
-        <v>240</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="E1:E81" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -4021,7 +4022,7 @@
   <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4035,19 +4036,19 @@
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>244</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>245</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>9</v>
@@ -4055,111 +4056,111 @@
     </row>
     <row r="2" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B2" s="6" t="s">
+        <v>245</v>
+      </c>
+      <c r="E2" s="6" t="s">
         <v>246</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="F2" s="6" t="s">
         <v>247</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B3" t="s">
+        <v>248</v>
+      </c>
+      <c r="D3" t="s">
         <v>249</v>
       </c>
-      <c r="D3" t="s">
-        <v>250</v>
-      </c>
       <c r="E3" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="4" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E4" s="6" t="s">
+        <v>246</v>
+      </c>
+      <c r="F4" s="6" t="s">
         <v>247</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B5" t="s">
+        <v>251</v>
+      </c>
+      <c r="D5" t="s">
         <v>252</v>
       </c>
-      <c r="D5" t="s">
-        <v>253</v>
-      </c>
       <c r="E5" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B6" t="s">
+        <v>253</v>
+      </c>
+      <c r="D6" t="s">
         <v>254</v>
       </c>
-      <c r="D6" t="s">
-        <v>255</v>
-      </c>
       <c r="E6" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="7" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E7" s="6" t="s">
+        <v>246</v>
+      </c>
+      <c r="F7" s="6" t="s">
         <v>247</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B8" t="s">
+        <v>256</v>
+      </c>
+      <c r="D8" t="s">
         <v>257</v>
       </c>
-      <c r="D8" t="s">
-        <v>258</v>
-      </c>
       <c r="E8" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B9" t="s">
+        <v>258</v>
+      </c>
+      <c r="D9" t="s">
         <v>259</v>
-      </c>
-      <c r="D9" t="s">
-        <v>260</v>
       </c>
       <c r="E9" t="s">
         <v>38</v>
@@ -4167,177 +4168,177 @@
     </row>
     <row r="10" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B10" s="6" t="s">
+        <v>260</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>246</v>
+      </c>
+      <c r="F10" s="6" t="s">
         <v>261</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>247</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>262</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B11" t="s">
+        <v>262</v>
+      </c>
+      <c r="D11" t="s">
         <v>263</v>
       </c>
-      <c r="D11" t="s">
-        <v>264</v>
-      </c>
       <c r="E11" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B12" t="s">
+        <v>264</v>
+      </c>
+      <c r="D12" t="s">
         <v>265</v>
       </c>
-      <c r="D12" t="s">
-        <v>266</v>
-      </c>
       <c r="E12" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="13" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B14" t="s">
+        <v>267</v>
+      </c>
+      <c r="D14" t="s">
         <v>268</v>
       </c>
-      <c r="D14" t="s">
-        <v>269</v>
-      </c>
       <c r="E14" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="15" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B16" t="s">
+        <v>270</v>
+      </c>
+      <c r="D16" t="s">
         <v>271</v>
-      </c>
-      <c r="D16" t="s">
-        <v>272</v>
       </c>
       <c r="E16" t="s">
         <v>121</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="17" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B17" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="D17" s="6" t="s">
         <v>274</v>
       </c>
-      <c r="D17" s="6" t="s">
-        <v>275</v>
-      </c>
       <c r="E17" s="6" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>275</v>
+      </c>
+      <c r="B19" t="s">
         <v>276</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>277</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>278</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
+        <v>167</v>
+      </c>
+      <c r="F19" t="s">
         <v>279</v>
-      </c>
-      <c r="E19" t="s">
-        <v>168</v>
-      </c>
-      <c r="F19" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B20" t="s">
+        <v>280</v>
+      </c>
+      <c r="C20" t="s">
+        <v>16</v>
+      </c>
+      <c r="D20" t="s">
         <v>281</v>
       </c>
-      <c r="C20" t="s">
-        <v>16</v>
-      </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
+        <v>176</v>
+      </c>
+      <c r="F20" t="s">
         <v>282</v>
-      </c>
-      <c r="E20" t="s">
-        <v>177</v>
-      </c>
-      <c r="F20" t="s">
-        <v>283</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B21" t="s">
+        <v>283</v>
+      </c>
+      <c r="C21" t="s">
         <v>284</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>285</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
+        <v>143</v>
+      </c>
+      <c r="F21" t="s">
         <v>286</v>
-      </c>
-      <c r="E21" t="s">
-        <v>144</v>
-      </c>
-      <c r="F21" t="s">
-        <v>287</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -4345,19 +4346,19 @@
         <v>10</v>
       </c>
       <c r="B23" t="s">
+        <v>287</v>
+      </c>
+      <c r="C23" t="s">
+        <v>277</v>
+      </c>
+      <c r="D23" t="s">
         <v>288</v>
       </c>
-      <c r="C23" t="s">
-        <v>278</v>
-      </c>
-      <c r="D23" t="s">
+      <c r="E23" t="s">
+        <v>140</v>
+      </c>
+      <c r="F23" t="s">
         <v>289</v>
-      </c>
-      <c r="E23" t="s">
-        <v>141</v>
-      </c>
-      <c r="F23" t="s">
-        <v>290</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -4365,19 +4366,19 @@
         <v>10</v>
       </c>
       <c r="B24" t="s">
+        <v>290</v>
+      </c>
+      <c r="C24" t="s">
+        <v>277</v>
+      </c>
+      <c r="D24" t="s">
         <v>291</v>
-      </c>
-      <c r="C24" t="s">
-        <v>278</v>
-      </c>
-      <c r="D24" t="s">
-        <v>292</v>
       </c>
       <c r="E24" t="s">
         <v>131</v>
       </c>
       <c r="F24" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -4385,10 +4386,10 @@
         <v>10</v>
       </c>
       <c r="B25" t="s">
+        <v>293</v>
+      </c>
+      <c r="D25" t="s">
         <v>294</v>
-      </c>
-      <c r="D25" t="s">
-        <v>295</v>
       </c>
       <c r="E25" s="7" t="s">
         <v>139</v>
@@ -4399,13 +4400,13 @@
         <v>10</v>
       </c>
       <c r="B26" t="s">
+        <v>295</v>
+      </c>
+      <c r="D26" t="s">
         <v>296</v>
       </c>
-      <c r="D26" t="s">
+      <c r="E26" t="s">
         <v>297</v>
-      </c>
-      <c r="E26" t="s">
-        <v>298</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -4413,19 +4414,19 @@
         <v>10</v>
       </c>
       <c r="B27" t="s">
+        <v>298</v>
+      </c>
+      <c r="C27" t="s">
         <v>299</v>
       </c>
-      <c r="C27" t="s">
+      <c r="D27" t="s">
         <v>300</v>
       </c>
-      <c r="D27" t="s">
+      <c r="E27" t="s">
         <v>301</v>
       </c>
-      <c r="E27" t="s">
-        <v>302</v>
-      </c>
       <c r="F27" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="28" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -4433,16 +4434,16 @@
         <v>10</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E28" s="6" t="s">
         <v>100</v>
       </c>
       <c r="F28" s="8" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
   </sheetData>
@@ -4451,6 +4452,34 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="3f138cb8-bfa4-4202-a7d1-f5ebc74c12f8">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="5c7ce210-0609-4e94-acf8-7b72a640ef35" xsi:nil="true"/>
+    <MediaLengthInSeconds xmlns="3f138cb8-bfa4-4202-a7d1-f5ebc74c12f8" xsi:nil="true"/>
+    <SharedWithUsers xmlns="5c7ce210-0609-4e94-acf8-7b72a640ef35">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000B2C28C9DB734A42B050F2647DD78F92" ma:contentTypeVersion="20" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="710ac9395ac8d6f4fd8fe072ea86a3d1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3f138cb8-bfa4-4202-a7d1-f5ebc74c12f8" xmlns:ns3="5c7ce210-0609-4e94-acf8-7b72a640ef35" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9da888daffaab2d6ca12ed91fa6262e8" ns2:_="" ns3:_="">
     <xsd:import namespace="3f138cb8-bfa4-4202-a7d1-f5ebc74c12f8"/>
@@ -4705,35 +4734,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC5EA8D3-22F0-4585-AA53-3CE2826CBDB6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="3f138cb8-bfa4-4202-a7d1-f5ebc74c12f8"/>
+    <ds:schemaRef ds:uri="5c7ce210-0609-4e94-acf8-7b72a640ef35"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="3f138cb8-bfa4-4202-a7d1-f5ebc74c12f8">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="5c7ce210-0609-4e94-acf8-7b72a640ef35" xsi:nil="true"/>
-    <MediaLengthInSeconds xmlns="3f138cb8-bfa4-4202-a7d1-f5ebc74c12f8" xsi:nil="true"/>
-    <SharedWithUsers xmlns="5c7ce210-0609-4e94-acf8-7b72a640ef35">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{65DB56A2-443E-4F9C-9692-D5CA8B5310D6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9B85F7D2-84CC-47B8-A6D2-93535A664907}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4750,23 +4770,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{65DB56A2-443E-4F9C-9692-D5CA8B5310D6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC5EA8D3-22F0-4585-AA53-3CE2826CBDB6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="3f138cb8-bfa4-4202-a7d1-f5ebc74c12f8"/>
-    <ds:schemaRef ds:uri="5c7ce210-0609-4e94-acf8-7b72a640ef35"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Alle karteringen kunnen door Veg2Hab v0.1
</commit_message>
<xml_diff>
--- a/data/Overzicht_vegetatiekarteringen.xlsx
+++ b/data/Overzicht_vegetatiekarteringen.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\jordydelange\git\veg2hab\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ABB8C2E-0059-468F-9E97-B8078804FE3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3E8357B-3E02-4D92-BE7F-82552B100682}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="27885" yWindow="1365" windowWidth="14985" windowHeight="15750" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4245" yWindow="4245" windowWidth="27150" windowHeight="15165" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Vegetatiekarteringen" sheetId="1" r:id="rId1"/>
@@ -707,9 +707,6 @@
     <t>Grote_Wielen_2013</t>
   </si>
   <si>
-    <t>./FR/Grote_Wielen_2013/vegetatietypen_Grutte_Wielen.shp</t>
-  </si>
-  <si>
     <t>SBB, (VvN)</t>
   </si>
   <si>
@@ -1089,6 +1086,9 @@
   </si>
   <si>
     <t>./DR Extra/2020_Drouwenerzand/HDL_Drouwenerzand_2020.shp</t>
+  </si>
+  <si>
+    <t>./FR/Grote_Wielen/Grote_Wielen_2013/vegetatietypen_Grutte_Wielen.shp</t>
   </si>
 </sst>
 </file>
@@ -1528,8 +1528,8 @@
   <dimension ref="A1:J81"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C45" sqref="C45"/>
+      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C58" sqref="C58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2895,7 +2895,7 @@
         <v>139</v>
       </c>
       <c r="C45" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D45" t="s">
         <v>13</v>
@@ -3241,7 +3241,7 @@
         <v>174</v>
       </c>
       <c r="C56" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D56" t="s">
         <v>13</v>
@@ -3305,7 +3305,7 @@
         <v>179</v>
       </c>
       <c r="C58" t="s">
-        <v>180</v>
+        <v>307</v>
       </c>
       <c r="D58" s="5" t="s">
         <v>13</v>
@@ -3314,19 +3314,19 @@
         <v>145</v>
       </c>
       <c r="F58" t="s">
+        <v>180</v>
+      </c>
+      <c r="G58" t="s">
+        <v>13</v>
+      </c>
+      <c r="H58" t="s">
+        <v>13</v>
+      </c>
+      <c r="I58" t="s">
+        <v>16</v>
+      </c>
+      <c r="J58" s="2" t="s">
         <v>181</v>
-      </c>
-      <c r="G58" t="s">
-        <v>13</v>
-      </c>
-      <c r="H58" t="s">
-        <v>13</v>
-      </c>
-      <c r="I58" t="s">
-        <v>16</v>
-      </c>
-      <c r="J58" s="2" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
@@ -3334,10 +3334,10 @@
         <v>142</v>
       </c>
       <c r="B59" t="s">
+        <v>182</v>
+      </c>
+      <c r="C59" t="s">
         <v>183</v>
-      </c>
-      <c r="C59" t="s">
-        <v>184</v>
       </c>
       <c r="D59" t="s">
         <v>13</v>
@@ -3363,10 +3363,10 @@
         <v>142</v>
       </c>
       <c r="B60" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="C60" s="4" t="s">
         <v>185</v>
-      </c>
-      <c r="C60" s="4" t="s">
-        <v>186</v>
       </c>
       <c r="D60" s="4" t="s">
         <v>13</v>
@@ -3387,7 +3387,7 @@
         <v>16</v>
       </c>
       <c r="J60" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
@@ -3395,10 +3395,10 @@
         <v>142</v>
       </c>
       <c r="B61" t="s">
+        <v>187</v>
+      </c>
+      <c r="C61" t="s">
         <v>188</v>
-      </c>
-      <c r="C61" t="s">
-        <v>189</v>
       </c>
       <c r="D61" t="s">
         <v>13</v>
@@ -3424,10 +3424,10 @@
         <v>142</v>
       </c>
       <c r="B62" t="s">
+        <v>189</v>
+      </c>
+      <c r="C62" t="s">
         <v>190</v>
-      </c>
-      <c r="C62" t="s">
-        <v>191</v>
       </c>
       <c r="D62" t="s">
         <v>13</v>
@@ -3453,10 +3453,10 @@
         <v>142</v>
       </c>
       <c r="B63" t="s">
+        <v>191</v>
+      </c>
+      <c r="C63" t="s">
         <v>192</v>
-      </c>
-      <c r="C63" t="s">
-        <v>193</v>
       </c>
       <c r="D63" t="s">
         <v>13</v>
@@ -3482,10 +3482,10 @@
         <v>142</v>
       </c>
       <c r="B64" t="s">
+        <v>193</v>
+      </c>
+      <c r="C64" t="s">
         <v>194</v>
-      </c>
-      <c r="C64" t="s">
-        <v>195</v>
       </c>
       <c r="D64" t="s">
         <v>13</v>
@@ -3506,18 +3506,18 @@
         <v>16</v>
       </c>
       <c r="J64" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
+        <v>196</v>
+      </c>
+      <c r="B65" t="s">
         <v>197</v>
       </c>
-      <c r="B65" t="s">
-        <v>198</v>
-      </c>
       <c r="C65" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D65" t="s">
         <v>13</v>
@@ -3540,13 +3540,13 @@
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B66" t="s">
+        <v>198</v>
+      </c>
+      <c r="C66" t="s">
         <v>199</v>
-      </c>
-      <c r="C66" t="s">
-        <v>200</v>
       </c>
       <c r="D66" t="s">
         <v>13</v>
@@ -3569,13 +3569,13 @@
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B67" t="s">
+        <v>200</v>
+      </c>
+      <c r="C67" t="s">
         <v>201</v>
-      </c>
-      <c r="C67" t="s">
-        <v>202</v>
       </c>
       <c r="D67" t="s">
         <v>13</v>
@@ -3598,13 +3598,13 @@
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B68" t="s">
+        <v>202</v>
+      </c>
+      <c r="C68" t="s">
         <v>203</v>
-      </c>
-      <c r="C68" t="s">
-        <v>204</v>
       </c>
       <c r="D68" t="s">
         <v>13</v>
@@ -3625,18 +3625,18 @@
         <v>16</v>
       </c>
       <c r="J68" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B69" t="s">
+        <v>205</v>
+      </c>
+      <c r="C69" t="s">
         <v>206</v>
-      </c>
-      <c r="C69" t="s">
-        <v>207</v>
       </c>
       <c r="D69" t="s">
         <v>13</v>
@@ -3662,27 +3662,27 @@
         <v>142</v>
       </c>
       <c r="B70" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="C70" s="4" t="s">
         <v>208</v>
       </c>
-      <c r="C70" s="4" t="s">
+      <c r="D70" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J70" s="4" t="s">
         <v>209</v>
-      </c>
-      <c r="D70" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J70" s="4" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="71" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="B71" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="B71" s="4" t="s">
+      <c r="C71" s="4" t="s">
         <v>212</v>
-      </c>
-      <c r="C71" s="4" t="s">
-        <v>213</v>
       </c>
       <c r="D71" s="4" t="s">
         <v>16</v>
@@ -3703,18 +3703,18 @@
         <v>16</v>
       </c>
       <c r="J71" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B72" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C72" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D72" t="s">
         <v>13</v>
@@ -3735,18 +3735,18 @@
         <v>13</v>
       </c>
       <c r="J72" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B73" t="s">
+        <v>216</v>
+      </c>
+      <c r="C73" t="s">
         <v>217</v>
-      </c>
-      <c r="C73" t="s">
-        <v>218</v>
       </c>
       <c r="D73" t="s">
         <v>13</v>
@@ -3767,18 +3767,18 @@
         <v>16</v>
       </c>
       <c r="J73" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B74" t="s">
+        <v>219</v>
+      </c>
+      <c r="C74" t="s">
         <v>220</v>
-      </c>
-      <c r="C74" t="s">
-        <v>221</v>
       </c>
       <c r="D74" t="s">
         <v>13</v>
@@ -3802,13 +3802,13 @@
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B75" t="s">
+        <v>221</v>
+      </c>
+      <c r="C75" t="s">
         <v>222</v>
-      </c>
-      <c r="C75" t="s">
-        <v>223</v>
       </c>
       <c r="D75" t="s">
         <v>13</v>
@@ -3831,13 +3831,13 @@
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B76" t="s">
+        <v>223</v>
+      </c>
+      <c r="C76" t="s">
         <v>224</v>
-      </c>
-      <c r="C76" t="s">
-        <v>225</v>
       </c>
       <c r="D76" t="s">
         <v>13</v>
@@ -3858,18 +3858,18 @@
         <v>13</v>
       </c>
       <c r="J76" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B77" t="s">
+        <v>225</v>
+      </c>
+      <c r="C77" t="s">
         <v>226</v>
-      </c>
-      <c r="C77" t="s">
-        <v>227</v>
       </c>
       <c r="D77" t="s">
         <v>13</v>
@@ -3892,13 +3892,13 @@
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B78" t="s">
+        <v>227</v>
+      </c>
+      <c r="C78" t="s">
         <v>228</v>
-      </c>
-      <c r="C78" t="s">
-        <v>229</v>
       </c>
       <c r="D78" t="s">
         <v>13</v>
@@ -3919,18 +3919,18 @@
         <v>13</v>
       </c>
       <c r="J78" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B79" t="s">
+        <v>230</v>
+      </c>
+      <c r="C79" t="s">
         <v>231</v>
-      </c>
-      <c r="C79" t="s">
-        <v>232</v>
       </c>
       <c r="D79" t="s">
         <v>13</v>
@@ -3953,39 +3953,39 @@
     </row>
     <row r="80" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80" s="4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B80" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="C80" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="C80" s="4" t="s">
+      <c r="D80" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G80" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H80" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I80" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J80" s="4" t="s">
         <v>234</v>
-      </c>
-      <c r="D80" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G80" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H80" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="I80" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J80" s="4" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="81" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B81" s="4" t="s">
+        <v>235</v>
+      </c>
+      <c r="C81" s="4" t="s">
         <v>236</v>
-      </c>
-      <c r="C81" s="4" t="s">
-        <v>237</v>
       </c>
       <c r="D81" s="4" t="s">
         <v>13</v>
@@ -3994,19 +3994,19 @@
         <v>66</v>
       </c>
       <c r="F81" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="G81" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H81" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I81" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J81" s="4" t="s">
         <v>238</v>
-      </c>
-      <c r="G81" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H81" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="I81" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J81" s="4" t="s">
-        <v>239</v>
       </c>
     </row>
   </sheetData>
@@ -4036,19 +4036,19 @@
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>243</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>244</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>9</v>
@@ -4056,111 +4056,111 @@
     </row>
     <row r="2" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B2" s="6" t="s">
+        <v>244</v>
+      </c>
+      <c r="E2" s="6" t="s">
         <v>245</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="F2" s="6" t="s">
         <v>246</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B3" t="s">
+        <v>247</v>
+      </c>
+      <c r="D3" t="s">
         <v>248</v>
       </c>
-      <c r="D3" t="s">
-        <v>249</v>
-      </c>
       <c r="E3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="4" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E4" s="6" t="s">
+        <v>245</v>
+      </c>
+      <c r="F4" s="6" t="s">
         <v>246</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B5" t="s">
+        <v>250</v>
+      </c>
+      <c r="D5" t="s">
         <v>251</v>
       </c>
-      <c r="D5" t="s">
-        <v>252</v>
-      </c>
       <c r="E5" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B6" t="s">
+        <v>252</v>
+      </c>
+      <c r="D6" t="s">
         <v>253</v>
       </c>
-      <c r="D6" t="s">
-        <v>254</v>
-      </c>
       <c r="E6" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="7" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E7" s="6" t="s">
+        <v>245</v>
+      </c>
+      <c r="F7" s="6" t="s">
         <v>246</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B8" t="s">
+        <v>255</v>
+      </c>
+      <c r="D8" t="s">
         <v>256</v>
       </c>
-      <c r="D8" t="s">
-        <v>257</v>
-      </c>
       <c r="E8" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B9" t="s">
+        <v>257</v>
+      </c>
+      <c r="D9" t="s">
         <v>258</v>
-      </c>
-      <c r="D9" t="s">
-        <v>259</v>
       </c>
       <c r="E9" t="s">
         <v>38</v>
@@ -4168,177 +4168,177 @@
     </row>
     <row r="10" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B10" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>245</v>
+      </c>
+      <c r="F10" s="6" t="s">
         <v>260</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>246</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B11" t="s">
+        <v>261</v>
+      </c>
+      <c r="D11" t="s">
         <v>262</v>
       </c>
-      <c r="D11" t="s">
-        <v>263</v>
-      </c>
       <c r="E11" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B12" t="s">
+        <v>263</v>
+      </c>
+      <c r="D12" t="s">
         <v>264</v>
       </c>
-      <c r="D12" t="s">
-        <v>265</v>
-      </c>
       <c r="E12" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="13" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B14" t="s">
+        <v>266</v>
+      </c>
+      <c r="D14" t="s">
         <v>267</v>
       </c>
-      <c r="D14" t="s">
-        <v>268</v>
-      </c>
       <c r="E14" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="15" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B16" t="s">
+        <v>269</v>
+      </c>
+      <c r="D16" t="s">
         <v>270</v>
-      </c>
-      <c r="D16" t="s">
-        <v>271</v>
       </c>
       <c r="E16" t="s">
         <v>121</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="17" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B17" s="6" t="s">
+        <v>272</v>
+      </c>
+      <c r="D17" s="6" t="s">
         <v>273</v>
       </c>
-      <c r="D17" s="6" t="s">
-        <v>274</v>
-      </c>
       <c r="E17" s="6" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>274</v>
+      </c>
+      <c r="B19" t="s">
         <v>275</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>276</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>277</v>
-      </c>
-      <c r="D19" t="s">
-        <v>278</v>
       </c>
       <c r="E19" t="s">
         <v>167</v>
       </c>
       <c r="F19" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B20" t="s">
+        <v>279</v>
+      </c>
+      <c r="C20" t="s">
+        <v>16</v>
+      </c>
+      <c r="D20" t="s">
         <v>280</v>
-      </c>
-      <c r="C20" t="s">
-        <v>16</v>
-      </c>
-      <c r="D20" t="s">
-        <v>281</v>
       </c>
       <c r="E20" t="s">
         <v>176</v>
       </c>
       <c r="F20" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B21" t="s">
+        <v>282</v>
+      </c>
+      <c r="C21" t="s">
         <v>283</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>284</v>
-      </c>
-      <c r="D21" t="s">
-        <v>285</v>
       </c>
       <c r="E21" t="s">
         <v>143</v>
       </c>
       <c r="F21" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -4346,19 +4346,19 @@
         <v>10</v>
       </c>
       <c r="B23" t="s">
+        <v>286</v>
+      </c>
+      <c r="C23" t="s">
+        <v>276</v>
+      </c>
+      <c r="D23" t="s">
         <v>287</v>
-      </c>
-      <c r="C23" t="s">
-        <v>277</v>
-      </c>
-      <c r="D23" t="s">
-        <v>288</v>
       </c>
       <c r="E23" t="s">
         <v>140</v>
       </c>
       <c r="F23" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -4366,19 +4366,19 @@
         <v>10</v>
       </c>
       <c r="B24" t="s">
+        <v>289</v>
+      </c>
+      <c r="C24" t="s">
+        <v>276</v>
+      </c>
+      <c r="D24" t="s">
         <v>290</v>
-      </c>
-      <c r="C24" t="s">
-        <v>277</v>
-      </c>
-      <c r="D24" t="s">
-        <v>291</v>
       </c>
       <c r="E24" t="s">
         <v>131</v>
       </c>
       <c r="F24" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -4386,10 +4386,10 @@
         <v>10</v>
       </c>
       <c r="B25" t="s">
+        <v>292</v>
+      </c>
+      <c r="D25" t="s">
         <v>293</v>
-      </c>
-      <c r="D25" t="s">
-        <v>294</v>
       </c>
       <c r="E25" s="7" t="s">
         <v>139</v>
@@ -4400,13 +4400,13 @@
         <v>10</v>
       </c>
       <c r="B26" t="s">
+        <v>294</v>
+      </c>
+      <c r="D26" t="s">
         <v>295</v>
       </c>
-      <c r="D26" t="s">
+      <c r="E26" t="s">
         <v>296</v>
-      </c>
-      <c r="E26" t="s">
-        <v>297</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -4414,19 +4414,19 @@
         <v>10</v>
       </c>
       <c r="B27" t="s">
+        <v>297</v>
+      </c>
+      <c r="C27" t="s">
         <v>298</v>
       </c>
-      <c r="C27" t="s">
+      <c r="D27" t="s">
         <v>299</v>
       </c>
-      <c r="D27" t="s">
+      <c r="E27" t="s">
         <v>300</v>
       </c>
-      <c r="E27" t="s">
-        <v>301</v>
-      </c>
       <c r="F27" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="28" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -4434,16 +4434,16 @@
         <v>10</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E28" s="6" t="s">
         <v>100</v>
       </c>
       <c r="F28" s="8" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
testing in place, spreadsheets edited
</commit_message>
<xml_diff>
--- a/data/Overzicht_vegetatiekarteringen.xlsx
+++ b/data/Overzicht_vegetatiekarteringen.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\jordydelange\git\veg2hab\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5756F26-F70E-4493-8C9B-AC9958F960BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DA4CB45-D324-4B0F-99ED-D65261133B4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="4245" yWindow="4245" windowWidth="27150" windowHeight="15165" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25800" windowHeight="21150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Vegetatiekarteringen" sheetId="1" r:id="rId1"/>
@@ -737,9 +737,6 @@
     <t>Sneekermeergebied_2009</t>
   </si>
   <si>
-    <t>./FR/Sneekermeergebied/Vegetatiekartering 2009/Structuur/Vegetatiekartering.shp</t>
-  </si>
-  <si>
     <t>Sneekermeergebied_2009_Terkaplester puollen</t>
   </si>
   <si>
@@ -1089,6 +1086,9 @@
   </si>
   <si>
     <t>./FR/Grote_Wielen/Grote_Wielen_2013/vegetatietypen_Grutte_Wielen.shp</t>
+  </si>
+  <si>
+    <t>./FR/Sneekermeergebied/Vegetatiekartering 2009/Snitsermar/vlakken.shp</t>
   </si>
 </sst>
 </file>
@@ -1525,18 +1525,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:J81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C41" sqref="C41"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Q19" sqref="Q19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.5703125" customWidth="1"/>
     <col min="2" max="2" width="56.28515625" customWidth="1"/>
-    <col min="3" max="3" width="68.42578125" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" customWidth="1"/>
     <col min="4" max="4" width="6.42578125" customWidth="1"/>
     <col min="5" max="5" width="18.7109375" customWidth="1"/>
     <col min="6" max="6" width="15.42578125" customWidth="1"/>
@@ -1577,7 +1578,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -1606,7 +1607,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -1638,7 +1639,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -1670,7 +1671,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -1702,7 +1703,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -1731,7 +1732,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -1763,7 +1764,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -1809,7 +1810,7 @@
         <v>13</v>
       </c>
       <c r="E9" t="s">
-        <v>14</v>
+        <v>66</v>
       </c>
       <c r="F9" t="s">
         <v>40</v>
@@ -1824,7 +1825,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -1856,7 +1857,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -1888,7 +1889,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -1917,7 +1918,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -1949,7 +1950,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -1981,7 +1982,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>10</v>
       </c>
@@ -2024,7 +2025,7 @@
         <v>13</v>
       </c>
       <c r="E16" t="s">
-        <v>14</v>
+        <v>66</v>
       </c>
       <c r="F16" t="s">
         <v>62</v>
@@ -2088,7 +2089,7 @@
         <v>13</v>
       </c>
       <c r="E18" t="s">
-        <v>14</v>
+        <v>66</v>
       </c>
       <c r="F18" t="s">
         <v>40</v>
@@ -2117,7 +2118,7 @@
         <v>13</v>
       </c>
       <c r="E19" t="s">
-        <v>14</v>
+        <v>66</v>
       </c>
       <c r="F19" t="s">
         <v>73</v>
@@ -2149,7 +2150,7 @@
         <v>13</v>
       </c>
       <c r="E20" t="s">
-        <v>14</v>
+        <v>66</v>
       </c>
       <c r="F20" t="s">
         <v>77</v>
@@ -2167,7 +2168,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>10</v>
       </c>
@@ -2210,7 +2211,7 @@
         <v>13</v>
       </c>
       <c r="E22" t="s">
-        <v>14</v>
+        <v>66</v>
       </c>
       <c r="F22" t="s">
         <v>77</v>
@@ -2242,7 +2243,7 @@
         <v>13</v>
       </c>
       <c r="E23" t="s">
-        <v>14</v>
+        <v>66</v>
       </c>
       <c r="F23" t="s">
         <v>40</v>
@@ -2257,7 +2258,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>86</v>
       </c>
@@ -2300,7 +2301,7 @@
         <v>13</v>
       </c>
       <c r="E25" t="s">
-        <v>14</v>
+        <v>66</v>
       </c>
       <c r="F25" t="s">
         <v>40</v>
@@ -2350,7 +2351,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="27" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>10</v>
       </c>
@@ -2405,7 +2406,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>10</v>
       </c>
@@ -2451,7 +2452,7 @@
         <v>13</v>
       </c>
       <c r="E30" t="s">
-        <v>14</v>
+        <v>66</v>
       </c>
       <c r="F30" t="s">
         <v>40</v>
@@ -2480,7 +2481,7 @@
         <v>13</v>
       </c>
       <c r="E31" t="s">
-        <v>14</v>
+        <v>66</v>
       </c>
       <c r="F31" t="s">
         <v>40</v>
@@ -2509,7 +2510,7 @@
         <v>13</v>
       </c>
       <c r="E32" t="s">
-        <v>14</v>
+        <v>66</v>
       </c>
       <c r="F32" t="s">
         <v>40</v>
@@ -2538,7 +2539,7 @@
         <v>13</v>
       </c>
       <c r="E33" t="s">
-        <v>14</v>
+        <v>66</v>
       </c>
       <c r="F33" t="s">
         <v>40</v>
@@ -2628,7 +2629,7 @@
         <v>13</v>
       </c>
       <c r="E36" t="s">
-        <v>14</v>
+        <v>66</v>
       </c>
       <c r="F36" t="s">
         <v>40</v>
@@ -2657,7 +2658,7 @@
         <v>13</v>
       </c>
       <c r="E37" t="s">
-        <v>14</v>
+        <v>66</v>
       </c>
       <c r="F37" t="s">
         <v>120</v>
@@ -2704,7 +2705,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>10</v>
       </c>
@@ -2736,7 +2737,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>10</v>
       </c>
@@ -2765,7 +2766,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>10</v>
       </c>
@@ -2808,7 +2809,7 @@
         <v>13</v>
       </c>
       <c r="E42" t="s">
-        <v>14</v>
+        <v>66</v>
       </c>
       <c r="F42" t="s">
         <v>40</v>
@@ -2840,7 +2841,7 @@
         <v>13</v>
       </c>
       <c r="E43" t="s">
-        <v>14</v>
+        <v>66</v>
       </c>
       <c r="F43" t="s">
         <v>120</v>
@@ -2855,7 +2856,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>10</v>
       </c>
@@ -2895,13 +2896,13 @@
         <v>139</v>
       </c>
       <c r="C45" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D45" t="s">
         <v>13</v>
       </c>
       <c r="E45" t="s">
-        <v>14</v>
+        <v>66</v>
       </c>
       <c r="F45" t="s">
         <v>67</v>
@@ -2916,7 +2917,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>86</v>
       </c>
@@ -2945,7 +2946,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>142</v>
       </c>
@@ -2977,7 +2978,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="48" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
         <v>142</v>
       </c>
@@ -3041,7 +3042,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>142</v>
       </c>
@@ -3105,7 +3106,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="52" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
         <v>142</v>
       </c>
@@ -3241,7 +3242,7 @@
         <v>174</v>
       </c>
       <c r="C56" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D56" t="s">
         <v>13</v>
@@ -3297,7 +3298,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>142</v>
       </c>
@@ -3305,7 +3306,7 @@
         <v>179</v>
       </c>
       <c r="C58" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D58" s="5" t="s">
         <v>13</v>
@@ -3329,7 +3330,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>142</v>
       </c>
@@ -3427,13 +3428,13 @@
         <v>189</v>
       </c>
       <c r="C62" t="s">
-        <v>190</v>
+        <v>307</v>
       </c>
       <c r="D62" t="s">
         <v>13</v>
       </c>
       <c r="E62" t="s">
-        <v>14</v>
+        <v>66</v>
       </c>
       <c r="F62" t="s">
         <v>40</v>
@@ -3453,10 +3454,10 @@
         <v>142</v>
       </c>
       <c r="B63" t="s">
+        <v>190</v>
+      </c>
+      <c r="C63" t="s">
         <v>191</v>
-      </c>
-      <c r="C63" t="s">
-        <v>192</v>
       </c>
       <c r="D63" t="s">
         <v>13</v>
@@ -3477,15 +3478,15 @@
         <v>16</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>142</v>
       </c>
       <c r="B64" t="s">
+        <v>192</v>
+      </c>
+      <c r="C64" t="s">
         <v>193</v>
-      </c>
-      <c r="C64" t="s">
-        <v>194</v>
       </c>
       <c r="D64" t="s">
         <v>13</v>
@@ -3506,18 +3507,18 @@
         <v>16</v>
       </c>
       <c r="J64" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
+        <v>195</v>
+      </c>
+      <c r="B65" t="s">
         <v>196</v>
       </c>
-      <c r="B65" t="s">
-        <v>197</v>
-      </c>
       <c r="C65" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D65" t="s">
         <v>13</v>
@@ -3540,13 +3541,13 @@
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B66" t="s">
+        <v>197</v>
+      </c>
+      <c r="C66" t="s">
         <v>198</v>
-      </c>
-      <c r="C66" t="s">
-        <v>199</v>
       </c>
       <c r="D66" t="s">
         <v>13</v>
@@ -3569,13 +3570,13 @@
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B67" t="s">
+        <v>199</v>
+      </c>
+      <c r="C67" t="s">
         <v>200</v>
-      </c>
-      <c r="C67" t="s">
-        <v>201</v>
       </c>
       <c r="D67" t="s">
         <v>13</v>
@@ -3598,13 +3599,13 @@
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B68" t="s">
+        <v>201</v>
+      </c>
+      <c r="C68" t="s">
         <v>202</v>
-      </c>
-      <c r="C68" t="s">
-        <v>203</v>
       </c>
       <c r="D68" t="s">
         <v>13</v>
@@ -3625,18 +3626,18 @@
         <v>16</v>
       </c>
       <c r="J68" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B69" t="s">
+        <v>204</v>
+      </c>
+      <c r="C69" t="s">
         <v>205</v>
-      </c>
-      <c r="C69" t="s">
-        <v>206</v>
       </c>
       <c r="D69" t="s">
         <v>13</v>
@@ -3657,32 +3658,32 @@
         <v>16</v>
       </c>
     </row>
-    <row r="70" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
         <v>142</v>
       </c>
       <c r="B70" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="C70" s="4" t="s">
         <v>207</v>
       </c>
-      <c r="C70" s="4" t="s">
+      <c r="D70" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J70" s="4" t="s">
         <v>208</v>
       </c>
-      <c r="D70" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J70" s="4" t="s">
+    </row>
+    <row r="71" spans="1:10" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="4" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="71" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="4" t="s">
+      <c r="B71" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="B71" s="4" t="s">
+      <c r="C71" s="4" t="s">
         <v>211</v>
-      </c>
-      <c r="C71" s="4" t="s">
-        <v>212</v>
       </c>
       <c r="D71" s="4" t="s">
         <v>16</v>
@@ -3703,18 +3704,18 @@
         <v>16</v>
       </c>
       <c r="J71" s="4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B72" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C72" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D72" t="s">
         <v>13</v>
@@ -3735,18 +3736,18 @@
         <v>13</v>
       </c>
       <c r="J72" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B73" t="s">
+        <v>215</v>
+      </c>
+      <c r="C73" t="s">
         <v>216</v>
-      </c>
-      <c r="C73" t="s">
-        <v>217</v>
       </c>
       <c r="D73" t="s">
         <v>13</v>
@@ -3767,18 +3768,18 @@
         <v>16</v>
       </c>
       <c r="J73" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B74" t="s">
+        <v>218</v>
+      </c>
+      <c r="C74" t="s">
         <v>219</v>
-      </c>
-      <c r="C74" t="s">
-        <v>220</v>
       </c>
       <c r="D74" t="s">
         <v>13</v>
@@ -3802,13 +3803,13 @@
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B75" t="s">
+        <v>220</v>
+      </c>
+      <c r="C75" t="s">
         <v>221</v>
-      </c>
-      <c r="C75" t="s">
-        <v>222</v>
       </c>
       <c r="D75" t="s">
         <v>13</v>
@@ -3831,19 +3832,19 @@
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B76" t="s">
+        <v>222</v>
+      </c>
+      <c r="C76" t="s">
         <v>223</v>
       </c>
-      <c r="C76" t="s">
-        <v>224</v>
-      </c>
       <c r="D76" t="s">
         <v>13</v>
       </c>
       <c r="E76" t="s">
-        <v>14</v>
+        <v>66</v>
       </c>
       <c r="F76" t="s">
         <v>40</v>
@@ -3858,18 +3859,18 @@
         <v>13</v>
       </c>
       <c r="J76" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B77" t="s">
+        <v>224</v>
+      </c>
+      <c r="C77" t="s">
         <v>225</v>
-      </c>
-      <c r="C77" t="s">
-        <v>226</v>
       </c>
       <c r="D77" t="s">
         <v>13</v>
@@ -3892,19 +3893,19 @@
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B78" t="s">
+        <v>226</v>
+      </c>
+      <c r="C78" t="s">
         <v>227</v>
       </c>
-      <c r="C78" t="s">
-        <v>228</v>
-      </c>
       <c r="D78" t="s">
         <v>13</v>
       </c>
       <c r="E78" t="s">
-        <v>14</v>
+        <v>66</v>
       </c>
       <c r="F78" t="s">
         <v>40</v>
@@ -3919,24 +3920,24 @@
         <v>13</v>
       </c>
       <c r="J78" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B79" t="s">
+        <v>229</v>
+      </c>
+      <c r="C79" t="s">
         <v>230</v>
       </c>
-      <c r="C79" t="s">
-        <v>231</v>
-      </c>
       <c r="D79" t="s">
         <v>13</v>
       </c>
       <c r="E79" t="s">
-        <v>14</v>
+        <v>66</v>
       </c>
       <c r="F79" t="s">
         <v>40</v>
@@ -3951,41 +3952,41 @@
         <v>16</v>
       </c>
     </row>
-    <row r="80" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" s="4" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B80" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="C80" s="4" t="s">
         <v>232</v>
       </c>
-      <c r="C80" s="4" t="s">
+      <c r="D80" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G80" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H80" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I80" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J80" s="4" t="s">
         <v>233</v>
-      </c>
-      <c r="D80" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G80" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H80" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="I80" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J80" s="4" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="81" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="4" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B81" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="C81" s="4" t="s">
         <v>235</v>
-      </c>
-      <c r="C81" s="4" t="s">
-        <v>236</v>
       </c>
       <c r="D81" s="4" t="s">
         <v>13</v>
@@ -3994,23 +3995,29 @@
         <v>66</v>
       </c>
       <c r="F81" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="G81" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H81" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I81" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J81" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="G81" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H81" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="I81" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J81" s="4" t="s">
-        <v>238</v>
-      </c>
     </row>
   </sheetData>
-  <autoFilter ref="E1:E81" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="E1:E81" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="access"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
@@ -4036,19 +4043,19 @@
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>242</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>243</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>9</v>
@@ -4056,111 +4063,111 @@
     </row>
     <row r="2" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B2" s="6" t="s">
+        <v>243</v>
+      </c>
+      <c r="E2" s="6" t="s">
         <v>244</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="F2" s="6" t="s">
         <v>245</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D3" t="s">
         <v>247</v>
       </c>
-      <c r="D3" t="s">
-        <v>248</v>
-      </c>
       <c r="E3" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="4" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E4" s="6" t="s">
+        <v>244</v>
+      </c>
+      <c r="F4" s="6" t="s">
         <v>245</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B5" t="s">
+        <v>249</v>
+      </c>
+      <c r="D5" t="s">
         <v>250</v>
       </c>
-      <c r="D5" t="s">
-        <v>251</v>
-      </c>
       <c r="E5" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B6" t="s">
+        <v>251</v>
+      </c>
+      <c r="D6" t="s">
         <v>252</v>
       </c>
-      <c r="D6" t="s">
-        <v>253</v>
-      </c>
       <c r="E6" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="7" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E7" s="6" t="s">
+        <v>244</v>
+      </c>
+      <c r="F7" s="6" t="s">
         <v>245</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B8" t="s">
+        <v>254</v>
+      </c>
+      <c r="D8" t="s">
         <v>255</v>
       </c>
-      <c r="D8" t="s">
-        <v>256</v>
-      </c>
       <c r="E8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B9" t="s">
+        <v>256</v>
+      </c>
+      <c r="D9" t="s">
         <v>257</v>
-      </c>
-      <c r="D9" t="s">
-        <v>258</v>
       </c>
       <c r="E9" t="s">
         <v>38</v>
@@ -4168,177 +4175,177 @@
     </row>
     <row r="10" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B10" s="6" t="s">
+        <v>258</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>244</v>
+      </c>
+      <c r="F10" s="6" t="s">
         <v>259</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>245</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B11" t="s">
+        <v>260</v>
+      </c>
+      <c r="D11" t="s">
         <v>261</v>
       </c>
-      <c r="D11" t="s">
-        <v>262</v>
-      </c>
       <c r="E11" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B12" t="s">
+        <v>262</v>
+      </c>
+      <c r="D12" t="s">
         <v>263</v>
       </c>
-      <c r="D12" t="s">
-        <v>264</v>
-      </c>
       <c r="E12" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="13" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B14" t="s">
+        <v>265</v>
+      </c>
+      <c r="D14" t="s">
         <v>266</v>
       </c>
-      <c r="D14" t="s">
-        <v>267</v>
-      </c>
       <c r="E14" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="15" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B16" t="s">
+        <v>268</v>
+      </c>
+      <c r="D16" t="s">
         <v>269</v>
-      </c>
-      <c r="D16" t="s">
-        <v>270</v>
       </c>
       <c r="E16" t="s">
         <v>121</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="17" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B17" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="D17" s="6" t="s">
         <v>272</v>
       </c>
-      <c r="D17" s="6" t="s">
-        <v>273</v>
-      </c>
       <c r="E17" s="6" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>273</v>
+      </c>
+      <c r="B19" t="s">
         <v>274</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>275</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>276</v>
-      </c>
-      <c r="D19" t="s">
-        <v>277</v>
       </c>
       <c r="E19" t="s">
         <v>167</v>
       </c>
       <c r="F19" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B20" t="s">
+        <v>278</v>
+      </c>
+      <c r="C20" t="s">
+        <v>16</v>
+      </c>
+      <c r="D20" t="s">
         <v>279</v>
-      </c>
-      <c r="C20" t="s">
-        <v>16</v>
-      </c>
-      <c r="D20" t="s">
-        <v>280</v>
       </c>
       <c r="E20" t="s">
         <v>176</v>
       </c>
       <c r="F20" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B21" t="s">
+        <v>281</v>
+      </c>
+      <c r="C21" t="s">
         <v>282</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>283</v>
-      </c>
-      <c r="D21" t="s">
-        <v>284</v>
       </c>
       <c r="E21" t="s">
         <v>143</v>
       </c>
       <c r="F21" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -4346,19 +4353,19 @@
         <v>10</v>
       </c>
       <c r="B23" t="s">
+        <v>285</v>
+      </c>
+      <c r="C23" t="s">
+        <v>275</v>
+      </c>
+      <c r="D23" t="s">
         <v>286</v>
-      </c>
-      <c r="C23" t="s">
-        <v>276</v>
-      </c>
-      <c r="D23" t="s">
-        <v>287</v>
       </c>
       <c r="E23" t="s">
         <v>140</v>
       </c>
       <c r="F23" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -4366,19 +4373,19 @@
         <v>10</v>
       </c>
       <c r="B24" t="s">
+        <v>288</v>
+      </c>
+      <c r="C24" t="s">
+        <v>275</v>
+      </c>
+      <c r="D24" t="s">
         <v>289</v>
-      </c>
-      <c r="C24" t="s">
-        <v>276</v>
-      </c>
-      <c r="D24" t="s">
-        <v>290</v>
       </c>
       <c r="E24" t="s">
         <v>131</v>
       </c>
       <c r="F24" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -4386,10 +4393,10 @@
         <v>10</v>
       </c>
       <c r="B25" t="s">
+        <v>291</v>
+      </c>
+      <c r="D25" t="s">
         <v>292</v>
-      </c>
-      <c r="D25" t="s">
-        <v>293</v>
       </c>
       <c r="E25" s="7" t="s">
         <v>139</v>
@@ -4400,13 +4407,13 @@
         <v>10</v>
       </c>
       <c r="B26" t="s">
+        <v>293</v>
+      </c>
+      <c r="D26" t="s">
         <v>294</v>
       </c>
-      <c r="D26" t="s">
+      <c r="E26" t="s">
         <v>295</v>
-      </c>
-      <c r="E26" t="s">
-        <v>296</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -4414,19 +4421,19 @@
         <v>10</v>
       </c>
       <c r="B27" t="s">
+        <v>296</v>
+      </c>
+      <c r="C27" t="s">
         <v>297</v>
       </c>
-      <c r="C27" t="s">
+      <c r="D27" t="s">
         <v>298</v>
       </c>
-      <c r="D27" t="s">
+      <c r="E27" t="s">
         <v>299</v>
       </c>
-      <c r="E27" t="s">
-        <v>300</v>
-      </c>
       <c r="F27" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="28" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -4434,16 +4441,16 @@
         <v>10</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="E28" s="6" t="s">
         <v>100</v>
       </c>
       <c r="F28" s="8" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
   </sheetData>
@@ -4452,34 +4459,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="3f138cb8-bfa4-4202-a7d1-f5ebc74c12f8">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="5c7ce210-0609-4e94-acf8-7b72a640ef35" xsi:nil="true"/>
-    <MediaLengthInSeconds xmlns="3f138cb8-bfa4-4202-a7d1-f5ebc74c12f8" xsi:nil="true"/>
-    <SharedWithUsers xmlns="5c7ce210-0609-4e94-acf8-7b72a640ef35">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000B2C28C9DB734A42B050F2647DD78F92" ma:contentTypeVersion="20" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="710ac9395ac8d6f4fd8fe072ea86a3d1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3f138cb8-bfa4-4202-a7d1-f5ebc74c12f8" xmlns:ns3="5c7ce210-0609-4e94-acf8-7b72a640ef35" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9da888daffaab2d6ca12ed91fa6262e8" ns2:_="" ns3:_="">
     <xsd:import namespace="3f138cb8-bfa4-4202-a7d1-f5ebc74c12f8"/>
@@ -4734,26 +4713,35 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC5EA8D3-22F0-4585-AA53-3CE2826CBDB6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="3f138cb8-bfa4-4202-a7d1-f5ebc74c12f8"/>
-    <ds:schemaRef ds:uri="5c7ce210-0609-4e94-acf8-7b72a640ef35"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{65DB56A2-443E-4F9C-9692-D5CA8B5310D6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="3f138cb8-bfa4-4202-a7d1-f5ebc74c12f8">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="5c7ce210-0609-4e94-acf8-7b72a640ef35" xsi:nil="true"/>
+    <MediaLengthInSeconds xmlns="3f138cb8-bfa4-4202-a7d1-f5ebc74c12f8" xsi:nil="true"/>
+    <SharedWithUsers xmlns="5c7ce210-0609-4e94-acf8-7b72a640ef35">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9B85F7D2-84CC-47B8-A6D2-93535A664907}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4770,4 +4758,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{65DB56A2-443E-4F9C-9692-D5CA8B5310D6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC5EA8D3-22F0-4585-AA53-3CE2826CBDB6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="3f138cb8-bfa4-4202-a7d1-f5ebc74c12f8"/>
+    <ds:schemaRef ds:uri="5c7ce210-0609-4e94-acf8-7b72a640ef35"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>